<commit_message>
Added support for description and acceptance criteria
</commit_message>
<xml_diff>
--- a/tickets_to_create.xlsx
+++ b/tickets_to_create.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Holden.holsinger\source\repos\jira_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6817F76D-B6FE-4B4E-9598-09E205C4CCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871E5EFA-8683-4695-B8AD-F4927A9755C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,26 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>issuetype</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>summary</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>GRW</t>
   </si>
   <si>
-    <t>Four score and seven years ago…</t>
-  </si>
-  <si>
-    <t>Lorem ipsum…</t>
-  </si>
-  <si>
     <t>Issue Type</t>
   </si>
   <si>
@@ -79,14 +64,59 @@
     <t>Sub-Task</t>
   </si>
   <si>
-    <t>simulates the epic</t>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - User Stories Only</t>
+  </si>
+  <si>
+    <t>Machine should dispense coffee without existential questioning. We need either an IT exorcism or a better espresso setup.</t>
+  </si>
+  <si>
+    <t>As a developer, I've noticed the office coffee machine now requires a secret handshake before dispensing caffeine. </t>
+  </si>
+  <si>
+    <t>As a consultant, I want my coffee to stay hot for longer than 10 minutes</t>
+  </si>
+  <si>
+    <t>As a consultant, I want meeting rooms to actually have chairs</t>
+  </si>
+  <si>
+    <t>Coffee remains at 140°F+ for at least 30 minutes after brewing</t>
+  </si>
+  <si>
+    <t>All meeting rooms have minimum 8 functional chairs rated for 8-hour workdays</t>
+  </si>
+  <si>
+    <t>DUMMY TICKET: Beverage Temperature Retention Enhancement</t>
+  </si>
+  <si>
+    <t>DUMMY TICKET: Meeting Room Seating Capacity Audit &amp; Restoration</t>
+  </si>
+  <si>
+    <t>DUMMY TICKET: Establish Conference Call Audio Clarity Protocol</t>
+  </si>
+  <si>
+    <t>As a consultant, I want to stop asking 'Can everyone hear me?' five times per call</t>
+  </si>
+  <si>
+    <t>Echo cancellation reduces repetitive "Can you hear me now?" questions by 90%</t>
+  </si>
+  <si>
+    <t>DUMMY EPIC: Fix Coffee Machine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +134,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -151,13 +189,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,63 +484,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -504,86 +595,86 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B6" s="3">
+        <v>10101</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B7" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B8" s="3">
         <v>14</v>
       </c>
-      <c r="B6" s="2">
-        <v>10101</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2">
-        <v>10000</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
functionality to link issues to epics
</commit_message>
<xml_diff>
--- a/tickets_to_create.xlsx
+++ b/tickets_to_create.xlsx
@@ -1,32 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Holden.holsinger\source\repos\jira_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871E5EFA-8683-4695-B8AD-F4927A9755C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827986F3-8D57-4A05-B8E5-26F6FC2128D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{DA255FFB-AB3C-470D-93CF-890D28C02D91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="info" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="config" sheetId="4" r:id="rId3"/>
+    <sheet name="info" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
   <si>
     <t>GRW</t>
   </si>
@@ -73,50 +89,80 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Acceptance Criteria - User Stories Only</t>
-  </si>
-  <si>
-    <t>Machine should dispense coffee without existential questioning. We need either an IT exorcism or a better espresso setup.</t>
-  </si>
-  <si>
-    <t>As a developer, I've noticed the office coffee machine now requires a secret handshake before dispensing caffeine. </t>
-  </si>
-  <si>
-    <t>As a consultant, I want my coffee to stay hot for longer than 10 minutes</t>
-  </si>
-  <si>
-    <t>As a consultant, I want meeting rooms to actually have chairs</t>
-  </si>
-  <si>
-    <t>Coffee remains at 140°F+ for at least 30 minutes after brewing</t>
-  </si>
-  <si>
-    <t>All meeting rooms have minimum 8 functional chairs rated for 8-hour workdays</t>
-  </si>
-  <si>
-    <t>DUMMY TICKET: Beverage Temperature Retention Enhancement</t>
-  </si>
-  <si>
-    <t>DUMMY TICKET: Meeting Room Seating Capacity Audit &amp; Restoration</t>
-  </si>
-  <si>
-    <t>DUMMY TICKET: Establish Conference Call Audio Clarity Protocol</t>
-  </si>
-  <si>
-    <t>As a consultant, I want to stop asking 'Can everyone hear me?' five times per call</t>
-  </si>
-  <si>
-    <t>Echo cancellation reduces repetitive "Can you hear me now?" questions by 90%</t>
-  </si>
-  <si>
-    <t>DUMMY EPIC: Fix Coffee Machine</t>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Onboarding Idea</t>
+  </si>
+  <si>
+    <t>ParentName</t>
+  </si>
+  <si>
+    <t>WorkType</t>
+  </si>
+  <si>
+    <t>Initiative</t>
+  </si>
+  <si>
+    <t>Work item ID</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Implements</t>
+  </si>
+  <si>
+    <t>Review Workspace</t>
+  </si>
+  <si>
+    <t>As the Product Manager for RW, I need to work with the SME group to define the high level components of their review process so that we can build the appropriate entities in Master Content Library (MCL) that will be required to execute the process in RW.</t>
+  </si>
+  <si>
+    <t>As a onboarding SME, I will populate the MCL Values workbook to define the applicable values and entity mappings for my review process so that these values can be imported into MCL to facilitate content definition.</t>
+  </si>
+  <si>
+    <t>As the Product Manager for RW, I need the values defined by the onboarding SMEs to be made available in MCL to facilitate the content build-out by the SMEs.</t>
+  </si>
+  <si>
+    <t>As an onboarding SME, I need to populate the MCL with all content required for the completion of my group's review process so that we can effeciently and accurately conduct review in RW.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add BUs relevant client types in the client types of drop-down field. The relationship between content type and client type will be the same as in MCL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add BUs relevant Sections and Categories in the scoping grid </t>
+  </si>
+  <si>
+    <t>The RW Team with work wiht the BU SME to create a Report Template. The template used is attached here IA Combined Review and Mock Report Template BU Version 1.docx and has comments and guidance on the data needed for the report. Following a similar format as the template, track changes is used to show new language and redlining to show language to be removed.</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>OnboardingIdea</t>
+  </si>
+  <si>
+    <t>PE-3985</t>
+  </si>
+  <si>
+    <t>Epic to link to / self</t>
+  </si>
+  <si>
+    <t>The RW Team with work with the BU SME to create a Report Template. The template used is attached here IA Combined Review and Mock Report Template BU Version 1.docx and has comments and guidance on the data needed for the report. Following a similar format as the template, track changes is used to show new language and redlining to show language to be removed.</t>
+  </si>
+  <si>
+    <t>RW: Configure and document new Review Workspace fields required for this Business Unit (e.g., business‑unit‑specific attributes, risk indicators, workflow flags), including defining field names and types, mapping to underlying data sources, updating screen/transition schemes, validating behavior in lower environments, and confirming with stakeholders that the configuration supports this Business Unit’s review, reporting, and controls requirements.</t>
+  </si>
+  <si>
+    <t>APS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +193,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -162,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,11 +238,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -200,10 +268,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,6 +292,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Template"/>
+      <sheetName val="Config"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>PE-3985</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,93 +592,377 @@
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Onboarding Kick-Off"</f>
+        <v>RW: APS - Onboarding Kick-Off</v>
+      </c>
+      <c r="D2" s="6" t="str">
+        <f>"Onboarding setup and kickoff operations for "&amp;config!A2</f>
+        <v>Onboarding setup and kickoff operations for APS</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - MCL Setup"</f>
+        <v>RW: APS - MCL Setup</v>
+      </c>
+      <c r="D3" s="6" t="str">
+        <f>"MCL Setup for "&amp;config!A2</f>
+        <v>MCL Setup for APS</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - RW Setup"</f>
+        <v>RW: APS - RW Setup</v>
+      </c>
+      <c r="D4" s="6" t="str">
+        <f>"RW Setup for "&amp;config!A2</f>
+        <v>RW Setup for APS</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Onboarding Launch"</f>
+        <v>RW: APS - Onboarding Launch</v>
+      </c>
+      <c r="D5" s="6" t="str">
+        <f>"Onboarding finalization and launch operations for "&amp;config!A2</f>
+        <v>Onboarding finalization and launch operations for APS</v>
+      </c>
+      <c r="E5" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Schedule Kick-Off Meeting"</f>
+        <v>RW: APS - Schedule Kick-Off Meeting</v>
+      </c>
+      <c r="D6" s="6" t="str">
+        <f>"As the Product Manager for RW, I want to meet with " &amp;config!A2&amp;" stakeholders to introduce them to the onboarding process and align on roles and expectations."</f>
+        <v>As the Product Manager for RW, I want to meet with APS stakeholders to introduce them to the onboarding process and align on roles and expectations.</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Establish SME List"</f>
+        <v>RW: APS - Establish SME List</v>
+      </c>
+      <c r="D7" s="6" t="str">
+        <f>"As the Product Manager for RW, I need to know which " &amp;config!A2&amp;" stakeholders will be actively participating in the onboarding process as group SMEs so that we can coordinate upcoming onboarding tasks and requirements sessions."</f>
+        <v>As the Product Manager for RW, I need to know which APS stakeholders will be actively participating in the onboarding process as group SMEs so that we can coordinate upcoming onboarding tasks and requirements sessions.</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Schedule SME Meeting"</f>
+        <v>RW: APS - Schedule SME Meeting</v>
+      </c>
+      <c r="D8" s="6" t="str">
+        <f>"As the Product Manager for RW, I want to meet with " &amp;config!A2&amp;" SMEs through scheduled meetings, so that I can understand their onboarding needs."</f>
+        <v>As the Product Manager for RW, I want to meet with APS SMEs through scheduled meetings, so that I can understand their onboarding needs.</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Define Review Components"</f>
+        <v>RW: APS - Define Review Components</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Define MCL Values"</f>
+        <v>RW: APS - Define MCL Values</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Load MCL Values"</f>
+        <v>RW: APS - Load MCL Values</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Populate MCL Content"</f>
+        <v>RW: APS - Populate MCL Content</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="E12" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="C13" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Create Content-Type"</f>
+        <v>RW: APS - Create Content-Type</v>
+      </c>
+      <c r="D13" s="6" t="str">
+        <f>"As an "&amp;config!A2&amp;" user, I need a content-type available in RW that corresponds with my team's review process so that we can configure the process to fit our needs without impacting other groups."</f>
+        <v>As an APS user, I need a content-type available in RW that corresponds with my team's review process so that we can configure the process to fit our needs without impacting other groups.</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="C14" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Configure Client Types"</f>
+        <v>RW: APS - Configure Client Types</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
+      <c r="C15" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Configure Section and Category Scoping"</f>
+        <v>RW: APS - Configure Section and Category Scoping</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>6</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Create Report Template"</f>
+        <v>RW: APS - Create Report Template</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>6</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Configure New RW Fields"</f>
+        <v>RW: APS - Configure New RW Fields</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>6</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Create Launch Plan"</f>
+        <v>RW: APS - Create Launch Plan</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f>"Develop and document a comprehensive launch plan for " &amp;config!A2&amp;_xlfn._LONGTEXT(" within Review Workspace, detailing objectives, scope, target users, timeline and milestones, stakeholder roles and responsibilities, communication and training plans, go‑live readiness checklist, and post‑launch monitoring to ensure a smooth and well‑coo","rdinated rollout.")</f>
+        <v>Develop and document a comprehensive launch plan for APS within Review Workspace, detailing objectives, scope, target users, timeline and milestones, stakeholder roles and responsibilities, communication and training plans, go‑live readiness checklist, and post‑launch monitoring to ensure a smooth and well‑coordinated rollout.</v>
+      </c>
+      <c r="E18" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Schedule Training"</f>
+        <v>RW: APS - Schedule Training</v>
+      </c>
+      <c r="D19" s="6" t="str">
+        <f>"Coordinate, schedule, and document " &amp;config!A2&amp;_xlfn._LONGTEXT(" training sessions for core user groups (reviewers, approvers, admins), including confirming objectives and audience, aligning on training materials and environment, sending invitations, and capturing attendance and follow‑ups to ensure users are prepared"," for go‑live.")</f>
+        <v>Coordinate, schedule, and document APS training sessions for core user groups (reviewers, approvers, admins), including confirming objectives and audience, aligning on training materials and environment, sending invitations, and capturing attendance and follow‑ups to ensure users are prepared for go‑live.</v>
+      </c>
+      <c r="E19" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>6</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7" t="str">
+        <f>"RW: "&amp;config!A2&amp;" - Create Post-Launch Support and Enhancement Agreement"</f>
+        <v>RW: APS - Create Post-Launch Support and Enhancement Agreement</v>
+      </c>
+      <c r="D20" s="6" t="str">
+        <f>"RW: Define and document a post‑launch support and enhancement agreement for " &amp;config!A2&amp;", covering ownership, SLAs, communication channels, release cadence, intake process for enhancements, escalation paths, and success metrics to ensure clear ongoing support after go‑live."</f>
+        <v>RW: Define and document a post‑launch support and enhancement agreement for APS, covering ownership, SLAs, communication channels, release cadence, intake process for enhancements, escalation paths, and success metrics to ensure clear ongoing support after go‑live.</v>
+      </c>
+      <c r="E20" s="6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -591,12 +972,758 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB8462D-2C23-4F0B-8245-5A6E4F29E98E}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B2" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="str">
+        <f>"RW: "&amp;A2&amp;" - Onboarding Kick-Off"</f>
+        <v>RW: APS - Onboarding Kick-Off</v>
+      </c>
+      <c r="F2" s="7" t="str">
+        <f>"Onboarding setup and kickoff operations for "&amp;A2</f>
+        <v>Onboarding setup and kickoff operations for APS</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B3" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="str">
+        <f>"RW: "&amp;A3&amp;" - MCL Setup"</f>
+        <v>RW: APS - MCL Setup</v>
+      </c>
+      <c r="F3" s="7" t="str">
+        <f>"MCL Setup for "&amp;A2</f>
+        <v>MCL Setup for APS</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="6">
+        <f>H2+1</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B4" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7" t="str">
+        <f>"RW: "&amp;A4&amp;" - RW Setup"</f>
+        <v>RW: APS - RW Setup</v>
+      </c>
+      <c r="F4" s="7" t="str">
+        <f>"RW Setup for "&amp;A2</f>
+        <v>RW Setup for APS</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:H20" si="0">H3+1</f>
+        <v>3</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="str">
+        <f>"RW: "&amp;A20&amp;" - Onboarding Launch"</f>
+        <v>RW: APS - Onboarding Launch</v>
+      </c>
+      <c r="F5" s="7" t="str">
+        <f>"Onboarding finalization and launch operations for "&amp;A2</f>
+        <v>Onboarding finalization and launch operations for APS</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B6" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f>"RW: "&amp;A6&amp;" - Onboarding Kick-Off"</f>
+        <v>RW: APS - Onboarding Kick-Off</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7" t="str">
+        <f>"RW: "&amp;A6&amp;" - Schedule Kick-Off Meeting"</f>
+        <v>RW: APS - Schedule Kick-Off Meeting</v>
+      </c>
+      <c r="F6" s="7" t="str">
+        <f>"As the Product Manager for RW, I want to meet with " &amp;A6&amp;" stakeholders to introduce them to the onboarding process and align on roles and expectations."</f>
+        <v>As the Product Manager for RW, I want to meet with APS stakeholders to introduce them to the onboarding process and align on roles and expectations.</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B7" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C7" s="7" t="str">
+        <f>"RW: "&amp;A7&amp;" - Onboarding Kick-Off"</f>
+        <v>RW: APS - Onboarding Kick-Off</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f>"RW: "&amp;A7&amp;" - Establish SME List"</f>
+        <v>RW: APS - Establish SME List</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f>"As the Product Manager for RW, I need to know which " &amp;A7&amp;" stakeholders will be actively participating in the onboarding process as group SMEs so that we can coordinate upcoming onboarding tasks and requirements sessions."</f>
+        <v>As the Product Manager for RW, I need to know which APS stakeholders will be actively participating in the onboarding process as group SMEs so that we can coordinate upcoming onboarding tasks and requirements sessions.</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C8" s="7" t="str">
+        <f>"RW: "&amp;A8&amp;" - Onboarding Kick-Off"</f>
+        <v>RW: APS - Onboarding Kick-Off</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7" t="str">
+        <f>"RW: "&amp;A8&amp;" - Schedule SME Meeting"</f>
+        <v>RW: APS - Schedule SME Meeting</v>
+      </c>
+      <c r="F8" s="7" t="str">
+        <f>"As the Product Manager for RW, I want to meet with " &amp;A8&amp;" SMEs through scheduled meetings, so that I can understand their onboarding needs."</f>
+        <v>As the Product Manager for RW, I want to meet with APS SMEs through scheduled meetings, so that I can understand their onboarding needs.</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B9" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C9" s="7" t="str">
+        <f>"RW: "&amp;A9&amp;" - MCL Setup"</f>
+        <v>RW: APS - MCL Setup</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7" t="str">
+        <f>"RW: "&amp;A8&amp;" - Define Review Components"</f>
+        <v>RW: APS - Define Review Components</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I9" s="6">
+        <v>2</v>
+      </c>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B10" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C10" s="7" t="str">
+        <f>"RW: "&amp;A10&amp;" - MCL Setup"</f>
+        <v>RW: APS - MCL Setup</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="7" t="str">
+        <f>"RW: "&amp;A9&amp;" - Define MCL Values"</f>
+        <v>RW: APS - Define MCL Values</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I10" s="6">
+        <v>2</v>
+      </c>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C11" s="7" t="str">
+        <f>"RW: "&amp;A11&amp;" - MCL Setup"</f>
+        <v>RW: APS - MCL Setup</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7" t="str">
+        <f>"RW: "&amp;A10&amp;" - Load MCL Values"</f>
+        <v>RW: APS - Load MCL Values</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I11" s="6">
+        <v>2</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B12" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C12" s="7" t="str">
+        <f>"RW: "&amp;A12&amp;" - MCL Setup"</f>
+        <v>RW: APS - MCL Setup</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="7" t="str">
+        <f>"RW: "&amp;A11&amp;" - Populate MCL Content"</f>
+        <v>RW: APS - Populate MCL Content</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I12" s="6">
+        <v>2</v>
+      </c>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B13" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C13" s="7" t="str">
+        <f>"RW: "&amp;A13&amp;" - RW Setup"</f>
+        <v>RW: APS - RW Setup</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="7" t="str">
+        <f>"RW: "&amp;A12&amp;" - Create Content-Type"</f>
+        <v>RW: APS - Create Content-Type</v>
+      </c>
+      <c r="F13" s="7" t="str">
+        <f>"As an "&amp;A6&amp;" user, I need a content-type available in RW that corresponds with my team's review process so that we can configure the process to fit our needs without impacting other groups."</f>
+        <v>As an APS user, I need a content-type available in RW that corresponds with my team's review process so that we can configure the process to fit our needs without impacting other groups.</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I13" s="6">
+        <v>3</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B14" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C14" s="7" t="str">
+        <f t="shared" ref="C14:C17" si="1">"RW: "&amp;A14&amp;" - RW Setup"</f>
+        <v>RW: APS - RW Setup</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="7" t="str">
+        <f>"RW: "&amp;A13&amp;" - Configure Client Types"</f>
+        <v>RW: APS - Configure Client Types</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="I14" s="6">
+        <v>3</v>
+      </c>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B15" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>RW: APS - RW Setup</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="7" t="str">
+        <f>"RW: "&amp;A14&amp;" - Configure Section and Category Scoping"</f>
+        <v>RW: APS - Configure Section and Category Scoping</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="I15" s="6">
+        <v>3</v>
+      </c>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B16" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C16" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>RW: APS - RW Setup</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="7" t="str">
+        <f>"RW: "&amp;A15&amp;" - Create Report Template"</f>
+        <v>RW: APS - Create Report Template</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="I16" s="6">
+        <v>3</v>
+      </c>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B17" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>RW: APS - RW Setup</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f>"RW: "&amp;A16&amp;" - Configure New RW Fields"</f>
+        <v>RW: APS - Configure New RW Fields</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="I17" s="6">
+        <v>3</v>
+      </c>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B18" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C18" s="7" t="str">
+        <f>"RW: "&amp;A18&amp;" - Onboarding Launch"</f>
+        <v>RW: APS - Onboarding Launch</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="7" t="str">
+        <f>"RW: "&amp;A17&amp;" - Create Launch Plan"</f>
+        <v>RW: APS - Create Launch Plan</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="I18" s="6">
+        <v>4</v>
+      </c>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B19" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C19" s="7" t="str">
+        <f>"RW: "&amp;A19&amp;" - Onboarding Launch"</f>
+        <v>RW: APS - Onboarding Launch</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7" t="str">
+        <f>"RW: "&amp;A18&amp;" - Schedule Training"</f>
+        <v>RW: APS - Schedule Training</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="I19" s="6">
+        <v>4</v>
+      </c>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="str">
+        <f>config!$A$2</f>
+        <v>APS</v>
+      </c>
+      <c r="B20" s="6" t="str">
+        <f>[1]Config!$B$2</f>
+        <v>PE-3985</v>
+      </c>
+      <c r="C20" s="7" t="str">
+        <f>"RW: "&amp;A20&amp;" - Onboarding Launch"</f>
+        <v>RW: APS - Onboarding Launch</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f>"RW: "&amp;A19&amp;" - Create Post-Launch Support and Enhancement Agreement"</f>
+        <v>RW: APS - Create Post-Launch Support and Enhancement Agreement</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="I20" s="6">
+        <v>4</v>
+      </c>
+      <c r="J20" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBF8C77-761D-45AB-900E-6112D43509B5}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442BC341-4204-429D-A45C-A1583D6CDD70}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>